<commit_message>
Updated with complete information
</commit_message>
<xml_diff>
--- a/OpenStack_Lab_Credentials.xlsx
+++ b/OpenStack_Lab_Credentials.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneCloud\openstack\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23117"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="40" yWindow="0" windowWidth="22440" windowHeight="13620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
   <si>
     <t>User1</t>
   </si>
@@ -51,6 +49,9 @@
   </si>
   <si>
     <t>User</t>
+  </si>
+  <si>
+    <t>AIO52</t>
   </si>
   <si>
     <t>AIO53</t>
@@ -111,6 +112,9 @@
     </r>
   </si>
   <si>
+    <t>10.1.64.152</t>
+  </si>
+  <si>
     <t>10.1.64.153</t>
   </si>
   <si>
@@ -345,43 +349,71 @@
     <t>VNC/RDP IP</t>
   </si>
   <si>
-    <r>
-      <t>AIO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>52</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>10.1.64.1</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>52</t>
-    </r>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>user12</t>
+  </si>
+  <si>
+    <t>user13</t>
+  </si>
+  <si>
+    <t>user14</t>
+  </si>
+  <si>
+    <t>user15</t>
+  </si>
+  <si>
+    <t>user16</t>
+  </si>
+  <si>
+    <t>66.220.11.249</t>
+  </si>
+  <si>
+    <t>sjc-0801</t>
+  </si>
+  <si>
+    <t>VNC Display</t>
+  </si>
+  <si>
+    <t>VNC Port</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +425,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -424,7 +472,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -447,11 +495,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,8 +540,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -537,7 +608,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,7 +643,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -749,7 +820,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -757,391 +828,589 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J2" sqref="J2:K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="12.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="23.5" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>5901</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="12"/>
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>5902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="12"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>5903</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="12"/>
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>5904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="12"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>5905</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>5906</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>5907</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>5908</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="12" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>5909</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="12"/>
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>5910</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="12"/>
       <c r="B12" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12">
+        <v>5911</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <v>5912</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="12"/>
       <c r="B14" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <v>5913</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>5914</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="12"/>
       <c r="B16" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <v>5915</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="12"/>
       <c r="B17" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+        <v>63</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J17">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <v>5916</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1149,6 +1418,11 @@
     <mergeCell ref="A10:A17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>